<commit_message>
final of the day commit
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamuelEke\Documents\UiPath\GitHub\fwf-Performer-DogCat-API\fwf-Performer-DogCatAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8569977A-B183-4556-8173-EA709C69F688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071F60A7-798B-4D01-9220-0346059EDF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="1545" windowWidth="19395" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -98,101 +98,121 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>pathToOutputReportData</t>
+  </si>
+  <si>
+    <t>Animal</t>
+  </si>
+  <si>
+    <t>pathToMapingEmployees</t>
+  </si>
+  <si>
+    <t>C:\Users\SamuelEke\Downloads\Mapare Mailuri.xlsx</t>
+  </si>
+  <si>
+    <t>cat,dog</t>
+  </si>
+  <si>
+    <t>CatAPI_URL</t>
+  </si>
+  <si>
+    <t>DogAPI_URL</t>
+  </si>
+  <si>
+    <t>https://cataas.com/cat</t>
+  </si>
+  <si>
+    <t>https://dog.ceo/api/breeds/image/random</t>
+  </si>
+  <si>
+    <t>emailSubject</t>
+  </si>
+  <si>
+    <t>Poze cu animale</t>
+  </si>
+  <si>
+    <t>pathToDownloadedImage</t>
+  </si>
+  <si>
+    <t>C:\Users\SamuelEke\Desktop\DogCat_API_Attachments</t>
+  </si>
+  <si>
+    <t>emailAddressOfManager</t>
+  </si>
+  <si>
+    <t>subjectForManager</t>
+  </si>
+  <si>
+    <t>Output Report Data</t>
+  </si>
+  <si>
+    <t>mail_folder_Path</t>
+  </si>
+  <si>
+    <t>apiDogs.Mail.Manager</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>MyQueueWithAnimals
-MyQueueWithAnimals
-MyQueueWithAnimals
-MyQueueWithAnimals</t>
-  </si>
-  <si>
-    <t>pathToOutputReportData</t>
-  </si>
-  <si>
-    <t>mail_folder_Path</t>
-  </si>
-  <si>
-    <t>Animal</t>
-  </si>
-  <si>
-    <t>pathToMapingEmployees</t>
-  </si>
-  <si>
-    <t>C:\Users\SamuelEke\Downloads\Mapare Mailuri.xlsx</t>
-  </si>
-  <si>
-    <t>cat,dog</t>
-  </si>
-  <si>
-    <t>CatAPI_URL</t>
-  </si>
-  <si>
-    <t>DogAPI_URL</t>
-  </si>
-  <si>
-    <t>https://cataas.com/cat</t>
-  </si>
-  <si>
-    <t>https://dog.ceo/api/breeds/image/random</t>
+  </si>
+  <si>
+    <t>MyQueueWithAnimals</t>
   </si>
 </sst>
 </file>
@@ -587,7 +607,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -634,10 +654,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -645,11 +665,11 @@
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -667,51 +687,74 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B15" s="2"/>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1694,7 +1737,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1747,18 +1790,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1782,7 +1825,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1804,7 +1847,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1815,7 +1858,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1826,62 +1869,62 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2864,7 +2907,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D9" sqref="D9:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2883,7 +2926,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2913,14 +2956,24 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="5"/>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Final touches to project.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamuelEke\Documents\UiPath\GitHub\fwf-Performer-DogCat-API\fwf-Performer-DogCatAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071F60A7-798B-4D01-9220-0346059EDF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECB06DC-3592-4E51-B4D5-F4A79E3A98B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -213,6 +213,13 @@
   </si>
   <si>
     <t>MyQueueWithAnimals</t>
+  </si>
+  <si>
+    <t>emailBody</t>
+  </si>
+  <si>
+    <t>What kind of tea is hard to swallow?
+Reality.</t>
   </si>
 </sst>
 </file>
@@ -606,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -743,7 +750,14 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2906,8 +2920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>